<commit_message>
Script 1 - atualização em 2025-09-06 02:14:47Z
</commit_message>
<xml_diff>
--- a/Data/g18.3.xlsx
+++ b/Data/g18.3.xlsx
@@ -740,13 +740,13 @@
         <v>2020</v>
       </c>
       <c r="B22" t="n">
-        <v>22.62864603422325</v>
+        <v>22.63496935893463</v>
       </c>
       <c r="C22" t="n">
-        <v>11.48600949732792</v>
+        <v>11.48367918335759</v>
       </c>
       <c r="D22" t="n">
-        <v>13.502228516036</v>
+        <v>13.5036084021264</v>
       </c>
     </row>
     <row r="23">
@@ -754,13 +754,13 @@
         <v>2021</v>
       </c>
       <c r="B23" t="n">
-        <v>23.09375128608094</v>
+        <v>23.10012769267524</v>
       </c>
       <c r="C23" t="n">
-        <v>11.83899338560302</v>
+        <v>11.8369437163957</v>
       </c>
       <c r="D23" t="n">
-        <v>13.73197279842373</v>
+        <v>13.73462385747906</v>
       </c>
     </row>
     <row r="24">
@@ -768,13 +768,13 @@
         <v>2022</v>
       </c>
       <c r="B24" t="n">
-        <v>23.52014634554608</v>
+        <v>23.52642530643275</v>
       </c>
       <c r="C24" t="n">
-        <v>12.16527192447055</v>
+        <v>12.16335479852913</v>
       </c>
       <c r="D24" t="n">
-        <v>13.9786838801615</v>
+        <v>13.98063481830828</v>
       </c>
     </row>
     <row r="25">
@@ -782,13 +782,13 @@
         <v>2023</v>
       </c>
       <c r="B25" t="n">
-        <v>23.70805016799442</v>
+        <v>23.71046689484384</v>
       </c>
       <c r="C25" t="n">
-        <v>12.4552971809046</v>
+        <v>12.45142418607468</v>
       </c>
       <c r="D25" t="n">
-        <v>14.00447811375554</v>
+        <v>14.00717120979344</v>
       </c>
     </row>
     <row r="26">
@@ -796,13 +796,13 @@
         <v>2024</v>
       </c>
       <c r="B26" t="n">
-        <v>23.92013904970397</v>
+        <v>23.91614243923391</v>
       </c>
       <c r="C26" t="n">
-        <v>12.6341692486481</v>
+        <v>12.62570199784373</v>
       </c>
       <c r="D26" t="n">
-        <v>14.1567870154906</v>
+        <v>14.15440654437449</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
atualização figuras do grupo 18.3 que tinha dado erro
</commit_message>
<xml_diff>
--- a/Data/g18.3.xlsx
+++ b/Data/g18.3.xlsx
@@ -740,13 +740,13 @@
         <v>2020</v>
       </c>
       <c r="B22" t="n">
-        <v>22.63496935893463</v>
+        <v>22.63548882549046</v>
       </c>
       <c r="C22" t="n">
-        <v>11.48367918335759</v>
+        <v>11.48481906767816</v>
       </c>
       <c r="D22" t="n">
-        <v>13.5036084021264</v>
+        <v>13.51093904698167</v>
       </c>
     </row>
     <row r="23">
@@ -754,13 +754,13 @@
         <v>2021</v>
       </c>
       <c r="B23" t="n">
-        <v>23.10012769267524</v>
+        <v>23.09893510493992</v>
       </c>
       <c r="C23" t="n">
-        <v>11.8369437163957</v>
+        <v>11.83471890624934</v>
       </c>
       <c r="D23" t="n">
-        <v>13.73462385747906</v>
+        <v>13.74061011986208</v>
       </c>
     </row>
     <row r="24">
@@ -768,13 +768,13 @@
         <v>2022</v>
       </c>
       <c r="B24" t="n">
-        <v>23.52642530643275</v>
+        <v>23.52577827880783</v>
       </c>
       <c r="C24" t="n">
-        <v>12.16335479852913</v>
+        <v>12.16101662962668</v>
       </c>
       <c r="D24" t="n">
-        <v>13.98063481830828</v>
+        <v>13.98682692633936</v>
       </c>
     </row>
     <row r="25">
@@ -782,13 +782,13 @@
         <v>2023</v>
       </c>
       <c r="B25" t="n">
-        <v>23.71046689484384</v>
+        <v>23.71146373109548</v>
       </c>
       <c r="C25" t="n">
-        <v>12.45142418607468</v>
+        <v>12.4483240726964</v>
       </c>
       <c r="D25" t="n">
-        <v>14.00717120979344</v>
+        <v>14.01600793116783</v>
       </c>
     </row>
     <row r="26">
@@ -796,13 +796,13 @@
         <v>2024</v>
       </c>
       <c r="B26" t="n">
-        <v>23.91614243923391</v>
+        <v>23.90207758604287</v>
       </c>
       <c r="C26" t="n">
-        <v>12.62570199784373</v>
+        <v>12.61414502123088</v>
       </c>
       <c r="D26" t="n">
-        <v>14.15440654437449</v>
+        <v>14.19608567023208</v>
       </c>
     </row>
   </sheetData>

</xml_diff>